<commit_message>
fix typo in mrs 277949 should be 277049
</commit_message>
<xml_diff>
--- a/src/main/resources/substituttlister/V16_manuelle_rullestoler_DK9.xlsx
+++ b/src/main/resources/substituttlister/V16_manuelle_rullestoler_DK9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinhanhtuantran/dev/navikt/hm/hm-grunndata-alternativprodukter/src/main/resources/substituttlister/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dinh.Anh.Tuan.Tran/dev/navikt/hm-grunndata-alternativprodukter/src/main/resources/substituttlister/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DA4068-D41C-884A-BAC6-6B98670825CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302281F6-FE69-6143-A4CC-5E0F5D44F405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="6500" windowWidth="38700" windowHeight="15380" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
+    <workbookView xWindow="53760" yWindow="3600" windowWidth="34560" windowHeight="15380" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -692,9 +692,6 @@
     <t>MRS komf Netti III HD sb55</t>
   </si>
   <si>
-    <t>277949</t>
-  </si>
-  <si>
     <t>219402</t>
   </si>
   <si>
@@ -720,6 +717,9 @@
   </si>
   <si>
     <t>316146</t>
+  </si>
+  <si>
+    <t>277049</t>
   </si>
 </sst>
 </file>
@@ -2190,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3485A8-7267-48FD-BE99-693AE922852B}">
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2370,10 +2370,10 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H19" s="23"/>
     </row>
@@ -2487,10 +2487,10 @@
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="H32" s="23"/>
     </row>
@@ -2622,16 +2622,16 @@
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="H47" s="23"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>56</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>57</v>
@@ -2838,7 +2838,7 @@
         <v>195</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H72" s="23"/>
     </row>
@@ -2847,7 +2847,7 @@
         <v>195</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H73" s="23"/>
     </row>
@@ -3003,7 +3003,7 @@
         <v>216</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H91" s="23"/>
     </row>
@@ -3012,7 +3012,7 @@
         <v>216</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="H92" s="23"/>
     </row>
@@ -3021,7 +3021,7 @@
         <v>216</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H93" s="23"/>
     </row>
@@ -3954,14 +3954,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a14b38d1-9dd6-42eb-8ce3-9f10d1a57fea" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="da616f65-0c92-4804-9f7f-4bb3cd0b0711">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4220,27 +4218,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a14b38d1-9dd6-42eb-8ce3-9f10d1a57fea" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="da616f65-0c92-4804-9f7f-4bb3cd0b0711">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDCCC35-05C9-417E-94AC-657FCAD914FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4408D7A9-E9B4-4E83-B739-4E128549896A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="da616f65-0c92-4804-9f7f-4bb3cd0b0711"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a14b38d1-9dd6-42eb-8ce3-9f10d1a57fea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4265,9 +4256,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4408D7A9-E9B4-4E83-B739-4E128549896A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDCCC35-05C9-417E-94AC-657FCAD914FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="da616f65-0c92-4804-9f7f-4bb3cd0b0711"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a14b38d1-9dd6-42eb-8ce3-9f10d1a57fea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>